<commit_message>
Meu amor está aqui hihihi
</commit_message>
<xml_diff>
--- a/Configuration Archive/ConfigArquivoLocalix.xlsx
+++ b/Configuration Archive/ConfigArquivoLocalix.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>NOM_VAR</t>
   </si>
@@ -127,12 +127,24 @@
   </si>
   <si>
     <t>SET</t>
+  </si>
+  <si>
+    <t>vUltimoMes</t>
+  </si>
+  <si>
+    <t>vMesAnterior</t>
+  </si>
+  <si>
+    <t>=monthname(maxstring(MES_ANO)-1)</t>
+  </si>
+  <si>
+    <t>=monthname(maxstring(MES_ANO))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -570,7 +582,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -614,58 +626,65 @@
     <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="22" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="26" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="30" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="34" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="19" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="23" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="27" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="31" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="35" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="39" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="20" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="24" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="28" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="32" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="36" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="40" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="17" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="21" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="25" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="29" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="33" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="37" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="6" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="10" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="12" builtinId="23" customBuiltin="1"/>
+  <cellStyles count="45">
+    <cellStyle name="20% - Ênfase1" xfId="18" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase2" xfId="22" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase3" xfId="26" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase4" xfId="30" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase5" xfId="34" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase6" xfId="38" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase1" xfId="19" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase2" xfId="23" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase3" xfId="27" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase4" xfId="31" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase5" xfId="35" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase6" xfId="39" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase1" xfId="20" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase2" xfId="24" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase3" xfId="28" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase4" xfId="32" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase5" xfId="36" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase6" xfId="40" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bom" xfId="5" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="10" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula de Verificação" xfId="12" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Célula Vinculada" xfId="11" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Comma 2" xfId="41"/>
-    <cellStyle name="Explanatory Text" xfId="15" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="5" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="3" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="4" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="8" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="7" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Ênfase1" xfId="17" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Ênfase2" xfId="21" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Ênfase3" xfId="25" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Ênfase4" xfId="29" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Ênfase5" xfId="33" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Ênfase6" xfId="37" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="8" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorreto" xfId="6" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutra" xfId="7" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="14" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="9" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Nota" xfId="14" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Saída" xfId="9" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de Aviso" xfId="13" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto Explicativo" xfId="15" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Title 2" xfId="42"/>
+    <cellStyle name="Título 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="2" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="3" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="4" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Título 5" xfId="44"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="13" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vírgula 2" xfId="43"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -681,7 +700,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -756,6 +775,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -791,6 +827,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -967,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,6 +1262,31 @@
       <c r="C21" s="2" t="s">
         <v>36</v>
       </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>